<commit_message>
Update DPW SUTAN IQBAL PRAMUDYA CHANDRA (3042019010).xlsx
</commit_message>
<xml_diff>
--- a/DPW SUTAN IQBAL PRAMUDYA CHANDRA (3042019010).xlsx
+++ b/DPW SUTAN IQBAL PRAMUDYA CHANDRA (3042019010).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\root\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\root\Downloads\UAS SUTAN IQBAL PRAMUDYA CHANDRA\uas_sipc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553D9EFF-2391-4734-8CBA-EE1DAABBFDE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A691E99F-2282-41B2-8A83-0376825DA7ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="10704" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>Sutan Iqbal Pramudya Chandra/3042019010</t>
   </si>
   <si>
-    <t>19010-sutaniqbal.uas.informatikapolitap.org</t>
+    <t>https://github.com/sutaniqbalpramudyachandra/uas_sipc</t>
   </si>
 </sst>
 </file>
@@ -228,9 +228,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -240,16 +237,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,16 +548,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -568,10 +568,10 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -579,13 +579,13 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -593,13 +593,13 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -607,13 +607,13 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -621,45 +621,45 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -667,10 +667,10 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1"/>
@@ -679,13 +679,13 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -693,13 +693,13 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -707,13 +707,13 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -721,13 +721,13 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -735,13 +735,13 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -749,10 +749,10 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="1"/>
@@ -761,13 +761,13 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -806,8 +806,9 @@
     <hyperlink ref="D11" r:id="rId22" xr:uid="{900572CE-A035-4230-A11A-1EB31B297776}"/>
     <hyperlink ref="D15" r:id="rId23" xr:uid="{BB884E7D-7EC9-4EE1-8E1D-2035D48860D6}"/>
     <hyperlink ref="D17" r:id="rId24" xr:uid="{EFCF6FEE-1117-4794-AF49-38824785F860}"/>
+    <hyperlink ref="C17" r:id="rId25" xr:uid="{300DE464-DDEC-406E-B03A-9F18CA114BCA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>